<commit_message>
[Cursor] Enhance fact extraction system with improved GUI and word-based chunking
- Updated chunking process to use words instead of characters (750 word chunks with 50 word overlaps)
- Completely redesigned GUI with tab-based interface for better visibility
- Added separate tabs for All Submissions, Approved Facts, Rejected Submissions, and Errors
- Fixed GUI Column parameter error by removing invalid 'label' parameter
- Changed terminology from "All Facts" to "All Submissions" for consistency
- Added real-time updates to all tabs during processing
- Improved error handling and display
- Added debug information for better troubleshooting
- Created test scripts to verify word-based chunking and GUI functionality
</commit_message>
<xml_diff>
--- a/facts.xlsx
+++ b/facts.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,7 +506,11 @@
           <t>SYNTHETIC_ARTICLE_6</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>The Future of Semiconductor Manufacturing: Innovation at the Atomic Scale
@@ -534,7 +538,11 @@
           <t>The submitted fact accurately reflects the specific achievement announced in the original text by TSMC regarding the demonstration of the world's first 1-nanometer process node. It includes two specific measurements: transistor density of 400 million transistors per square millimeter and power efficiency of 0.2 watts per million transistors. The fact maintains the complete technical context of the original statement, including the entity (TSMC) and the achieved metrics. All units are specified (transistors per square millimeter, watts per million transistors), and the conditions of the demonstration are preserved. There is no additional information or inference beyond what was explicitly stated in the original text.</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
@@ -549,6 +557,1095 @@
       <c r="L2" t="inlineStr">
         <is>
           <t>{"chunk_metadata": {"char_length": 2968, "timestamp": "2025-02-23T20:08:51.944499"}, "llm_response": "&lt;fact&gt;TSMC successfully demonstrated the world's first 1-nanometer process node, achieving a transistor density of 400 million transistors per square millimeter with a power efficiency of 0.2 watts per million transistors&lt;/fact&gt;\n&lt;fact&gt;The semiconductor industry has adopted extreme ultraviolet (EUV) lithography for patterning circuits onto silicon wafers&lt;/fact&gt;", "extraction_time": 1.281868, "extraction_model": "gpt-3.5-turbo", "fact_number": 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:08:59.553755</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NICHOLAS PATE 
+329 E 63rd, #3A | New York, NY 10065 
+Tel: 512-966-4317 | E-mail: nicholas.pate1320@gmail.com 
+EXPERIENCE 
+Dell Technologies 
+Corporate Strategy Consultant 
+New York, NY 
+Nov 2021 – Present 
+• Led AI strategy projects, scoping and structuring complex questions and executing hypotheses-driven frameworks 
+• Synthesized insights into internal and external collateral; delivered strategic recommendations to senior leadership 
+• Conducted primary market research and developed data-driven insights to inform AI growth strategies 
+• Developed and led AI training initiatives, including upskilling and thought leadership for Corporate Strategy team 
+• Delivered macroeconomic, business, and consumer insights to SVP and C-Suite executives to aid in annual planning 
+• Built relationships and collaborated effectively with colleagues at all levels to create and drive adoption of AI strategies 
+L.E.K. Consulting 
+Consultant 
+Summer Consultant 
+New York, NY 
+Jan 2021 – Oct 2021  
+Summer 2019 
+• Led and managed teams of 2-3 associates in the execution of commercial and vendor due diligence projects, providing 
+valuable insights for buy-side and sell-side transactions 
+• Developed and implemented hypothesis-led frameworks to provide comprehensive market dynamics insights, 
+including growth drivers, competitive landscapes, customer segmentation, unmet needs, and key purchasing criteria 
+• Conducted primary market research through the development of consumer surveys and interview guides, providing 
+data-driven insights to inform growth strategies 
+• Developed market size models to determine current market size and forecasted growth, aiding in strategic decision-
+making for clients across various industries 
+Grant Thornton LLP 
+Senior Associate Consultant – Strategy and Performance Improvement  
+Associate Consultant – Business Consulting (Dallas, TX) 
+New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Nicholas Pate worked as a Consultant at L.E.K. Consulting in New York, NY from Jan 2021 to Oct 2021</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>The submitted fact states that Nicholas Pate worked as a Consultant at L.E.K. Consulting in New York, NY from Jan 2021 to Oct 2021. This fact can be verified directly from the original text, which clearly mentions Nicholas Pate's experience at L.E.K. Consulting as a Consultant during the specified time period.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>3.974826</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 2286, "timestamp": "2025-02-24T00:08:55.555905"}, "llm_response": "&lt;fact&gt;Nicholas Pate's phone number is 512-966-4317&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate's email address is nicholas.pate1320@gmail.com&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Corporate Strategy Consultant at Dell Technologies in New York, NY from Nov 2021 to Present&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led AI strategy projects at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate conducted primary market research at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate developed and led AI training initiatives at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate delivered macroeconomic, business, and consumer insights to SVP and C-Suite executives at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Consultant at L.E.K. Consulting in New York, NY from Jan 2021 to Oct 2021&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led and managed teams of 2-3 associates at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate developed and implemented hypothesis-led frameworks at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate conducted primary market research through the development of consumer surveys and interview guides at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Senior Associate Consultant at Grant Thornton LLP in New York, NY from 2016 to 2018&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate consulted for 10+ clients over 4+ years at Grant Thornton LLP&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led data-driven projects using SQL analytics at Grant Thornton LLP&lt;/fact&gt;", "extraction_time": 3.974826, "extraction_model": "gpt-3.5-turbo", "fact_number": 8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:08:59.553765</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NICHOLAS PATE 
+329 E 63rd, #3A | New York, NY 10065 
+Tel: 512-966-4317 | E-mail: nicholas.pate1320@gmail.com 
+EXPERIENCE 
+Dell Technologies 
+Corporate Strategy Consultant 
+New York, NY 
+Nov 2021 – Present 
+• Led AI strategy projects, scoping and structuring complex questions and executing hypotheses-driven frameworks 
+• Synthesized insights into internal and external collateral; delivered strategic recommendations to senior leadership 
+• Conducted primary market research and developed data-driven insights to inform AI growth strategies 
+• Developed and led AI training initiatives, including upskilling and thought leadership for Corporate Strategy team 
+• Delivered macroeconomic, business, and consumer insights to SVP and C-Suite executives to aid in annual planning 
+• Built relationships and collaborated effectively with colleagues at all levels to create and drive adoption of AI strategies 
+L.E.K. Consulting 
+Consultant 
+Summer Consultant 
+New York, NY 
+Jan 2021 – Oct 2021  
+Summer 2019 
+• Led and managed teams of 2-3 associates in the execution of commercial and vendor due diligence projects, providing 
+valuable insights for buy-side and sell-side transactions 
+• Developed and implemented hypothesis-led frameworks to provide comprehensive market dynamics insights, 
+including growth drivers, competitive landscapes, customer segmentation, unmet needs, and key purchasing criteria 
+• Conducted primary market research through the development of consumer surveys and interview guides, providing 
+data-driven insights to inform growth strategies 
+• Developed market size models to determine current market size and forecasted growth, aiding in strategic decision-
+making for clients across various industries 
+Grant Thornton LLP 
+Senior Associate Consultant – Strategy and Performance Improvement  
+Associate Consultant – Business Consulting (Dallas, TX) 
+New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Nicholas Pate led and managed teams of 2-3 associates at L.E.K. Consulting</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>The submitted fact states that Nicholas Pate led and managed teams of 2-3 associates at L.E.K. Consulting. This fact can be verified directly from the original text in the experience section where it mentions that Nicholas Pate "Led and managed teams of 2-3 associates in the execution of commercial and vendor due diligence projects" during his time at L.E.K. Consulting. The fact preserves the specific number of associates (2-3) and the context of his role at the consulting firm.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>3.974826</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 2286, "timestamp": "2025-02-24T00:08:55.555905"}, "llm_response": "&lt;fact&gt;Nicholas Pate's phone number is 512-966-4317&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate's email address is nicholas.pate1320@gmail.com&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Corporate Strategy Consultant at Dell Technologies in New York, NY from Nov 2021 to Present&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led AI strategy projects at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate conducted primary market research at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate developed and led AI training initiatives at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate delivered macroeconomic, business, and consumer insights to SVP and C-Suite executives at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Consultant at L.E.K. Consulting in New York, NY from Jan 2021 to Oct 2021&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led and managed teams of 2-3 associates at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate developed and implemented hypothesis-led frameworks at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate conducted primary market research through the development of consumer surveys and interview guides at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Senior Associate Consultant at Grant Thornton LLP in New York, NY from 2016 to 2018&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate consulted for 10+ clients over 4+ years at Grant Thornton LLP&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led data-driven projects using SQL analytics at Grant Thornton LLP&lt;/fact&gt;", "extraction_time": 3.974826, "extraction_model": "gpt-3.5-turbo", "fact_number": 9}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:08:59.553788</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NICHOLAS PATE 
+329 E 63rd, #3A | New York, NY 10065 
+Tel: 512-966-4317 | E-mail: nicholas.pate1320@gmail.com 
+EXPERIENCE 
+Dell Technologies 
+Corporate Strategy Consultant 
+New York, NY 
+Nov 2021 – Present 
+• Led AI strategy projects, scoping and structuring complex questions and executing hypotheses-driven frameworks 
+• Synthesized insights into internal and external collateral; delivered strategic recommendations to senior leadership 
+• Conducted primary market research and developed data-driven insights to inform AI growth strategies 
+• Developed and led AI training initiatives, including upskilling and thought leadership for Corporate Strategy team 
+• Delivered macroeconomic, business, and consumer insights to SVP and C-Suite executives to aid in annual planning 
+• Built relationships and collaborated effectively with colleagues at all levels to create and drive adoption of AI strategies 
+L.E.K. Consulting 
+Consultant 
+Summer Consultant 
+New York, NY 
+Jan 2021 – Oct 2021  
+Summer 2019 
+• Led and managed teams of 2-3 associates in the execution of commercial and vendor due diligence projects, providing 
+valuable insights for buy-side and sell-side transactions 
+• Developed and implemented hypothesis-led frameworks to provide comprehensive market dynamics insights, 
+including growth drivers, competitive landscapes, customer segmentation, unmet needs, and key purchasing criteria 
+• Conducted primary market research through the development of consumer surveys and interview guides, providing 
+data-driven insights to inform growth strategies 
+• Developed market size models to determine current market size and forecasted growth, aiding in strategic decision-
+making for clients across various industries 
+Grant Thornton LLP 
+Senior Associate Consultant – Strategy and Performance Improvement  
+Associate Consultant – Business Consulting (Dallas, TX) 
+New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Nicholas Pate conducted primary market research through the development of consumer surveys and interview guides at L.E.K. Consulting</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>The submitted fact accurately reflects the original text. Nicholas Pate's involvement in conducting primary market research through the development of consumer surveys and interview guides at L.E.K. Consulting is explicitly mentioned in the provided text. The fact maintains the specific activity, context, and role performed by Nicholas Pate during his time at L.E.K. Consulting without adding any new information or making any inferences.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>3.974826</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 2286, "timestamp": "2025-02-24T00:08:55.555905"}, "llm_response": "&lt;fact&gt;Nicholas Pate's phone number is 512-966-4317&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate's email address is nicholas.pate1320@gmail.com&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Corporate Strategy Consultant at Dell Technologies in New York, NY from Nov 2021 to Present&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led AI strategy projects at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate conducted primary market research at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate developed and led AI training initiatives at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate delivered macroeconomic, business, and consumer insights to SVP and C-Suite executives at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Consultant at L.E.K. Consulting in New York, NY from Jan 2021 to Oct 2021&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led and managed teams of 2-3 associates at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate developed and implemented hypothesis-led frameworks at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate conducted primary market research through the development of consumer surveys and interview guides at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Senior Associate Consultant at Grant Thornton LLP in New York, NY from 2016 to 2018&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate consulted for 10+ clients over 4+ years at Grant Thornton LLP&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led data-driven projects using SQL analytics at Grant Thornton LLP&lt;/fact&gt;", "extraction_time": 3.974826, "extraction_model": "gpt-3.5-turbo", "fact_number": 11}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:08:59.553800</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NICHOLAS PATE 
+329 E 63rd, #3A | New York, NY 10065 
+Tel: 512-966-4317 | E-mail: nicholas.pate1320@gmail.com 
+EXPERIENCE 
+Dell Technologies 
+Corporate Strategy Consultant 
+New York, NY 
+Nov 2021 – Present 
+• Led AI strategy projects, scoping and structuring complex questions and executing hypotheses-driven frameworks 
+• Synthesized insights into internal and external collateral; delivered strategic recommendations to senior leadership 
+• Conducted primary market research and developed data-driven insights to inform AI growth strategies 
+• Developed and led AI training initiatives, including upskilling and thought leadership for Corporate Strategy team 
+• Delivered macroeconomic, business, and consumer insights to SVP and C-Suite executives to aid in annual planning 
+• Built relationships and collaborated effectively with colleagues at all levels to create and drive adoption of AI strategies 
+L.E.K. Consulting 
+Consultant 
+Summer Consultant 
+New York, NY 
+Jan 2021 – Oct 2021  
+Summer 2019 
+• Led and managed teams of 2-3 associates in the execution of commercial and vendor due diligence projects, providing 
+valuable insights for buy-side and sell-side transactions 
+• Developed and implemented hypothesis-led frameworks to provide comprehensive market dynamics insights, 
+including growth drivers, competitive landscapes, customer segmentation, unmet needs, and key purchasing criteria 
+• Conducted primary market research through the development of consumer surveys and interview guides, providing 
+data-driven insights to inform growth strategies 
+• Developed market size models to determine current market size and forecasted growth, aiding in strategic decision-
+making for clients across various industries 
+Grant Thornton LLP 
+Senior Associate Consultant – Strategy and Performance Improvement  
+Associate Consultant – Business Consulting (Dallas, TX) 
+New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Nicholas Pate worked as a Senior Associate Consultant at Grant Thornton LLP in New York, NY from 2016 to 2018</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>The submitted fact accurately reflects the information provided in the original text. It names the specific individual (Nicholas Pate), the position held (Senior Associate Consultant), the company (Grant Thornton LLP), the location (New York, NY), and the time frame (2016 - 2018). The fact contains specific, verifiable data points and maintains all the necessary details without adding any inference or additional information. It meets all the criteria for a valid fact based on the original text.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>3.974826</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 2286, "timestamp": "2025-02-24T00:08:55.555905"}, "llm_response": "&lt;fact&gt;Nicholas Pate's phone number is 512-966-4317&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate's email address is nicholas.pate1320@gmail.com&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Corporate Strategy Consultant at Dell Technologies in New York, NY from Nov 2021 to Present&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led AI strategy projects at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate conducted primary market research at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate developed and led AI training initiatives at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate delivered macroeconomic, business, and consumer insights to SVP and C-Suite executives at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Consultant at L.E.K. Consulting in New York, NY from Jan 2021 to Oct 2021&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led and managed teams of 2-3 associates at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate developed and implemented hypothesis-led frameworks at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate conducted primary market research through the development of consumer surveys and interview guides at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Senior Associate Consultant at Grant Thornton LLP in New York, NY from 2016 to 2018&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate consulted for 10+ clients over 4+ years at Grant Thornton LLP&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led data-driven projects using SQL analytics at Grant Thornton LLP&lt;/fact&gt;", "extraction_time": 3.974826, "extraction_model": "gpt-3.5-turbo", "fact_number": 12}</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:08:59.553821</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NICHOLAS PATE 
+329 E 63rd, #3A | New York, NY 10065 
+Tel: 512-966-4317 | E-mail: nicholas.pate1320@gmail.com 
+EXPERIENCE 
+Dell Technologies 
+Corporate Strategy Consultant 
+New York, NY 
+Nov 2021 – Present 
+• Led AI strategy projects, scoping and structuring complex questions and executing hypotheses-driven frameworks 
+• Synthesized insights into internal and external collateral; delivered strategic recommendations to senior leadership 
+• Conducted primary market research and developed data-driven insights to inform AI growth strategies 
+• Developed and led AI training initiatives, including upskilling and thought leadership for Corporate Strategy team 
+• Delivered macroeconomic, business, and consumer insights to SVP and C-Suite executives to aid in annual planning 
+• Built relationships and collaborated effectively with colleagues at all levels to create and drive adoption of AI strategies 
+L.E.K. Consulting 
+Consultant 
+Summer Consultant 
+New York, NY 
+Jan 2021 – Oct 2021  
+Summer 2019 
+• Led and managed teams of 2-3 associates in the execution of commercial and vendor due diligence projects, providing 
+valuable insights for buy-side and sell-side transactions 
+• Developed and implemented hypothesis-led frameworks to provide comprehensive market dynamics insights, 
+including growth drivers, competitive landscapes, customer segmentation, unmet needs, and key purchasing criteria 
+• Conducted primary market research through the development of consumer surveys and interview guides, providing 
+data-driven insights to inform growth strategies 
+• Developed market size models to determine current market size and forecasted growth, aiding in strategic decision-
+making for clients across various industries 
+Grant Thornton LLP 
+Senior Associate Consultant – Strategy and Performance Improvement  
+Associate Consultant – Business Consulting (Dallas, TX) 
+New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Nicholas Pate led data-driven projects using SQL analytics at Grant Thornton LLP</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>The submitted fact accurately reflects the original text. Nicholas Pate's role at Grant Thornton LLP included leading data-driven projects using SQL analytics, as stated in the text. This statement directly matches the information provided in the experience section of the original text without adding any new information or making any inferences. The fact contains a specific, measurable data point (use of SQL analytics) that can be independently verified through the original text.</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>3.974826</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 2286, "timestamp": "2025-02-24T00:08:55.555905"}, "llm_response": "&lt;fact&gt;Nicholas Pate's phone number is 512-966-4317&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate's email address is nicholas.pate1320@gmail.com&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Corporate Strategy Consultant at Dell Technologies in New York, NY from Nov 2021 to Present&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led AI strategy projects at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate conducted primary market research at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate developed and led AI training initiatives at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate delivered macroeconomic, business, and consumer insights to SVP and C-Suite executives at Dell Technologies&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Consultant at L.E.K. Consulting in New York, NY from Jan 2021 to Oct 2021&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led and managed teams of 2-3 associates at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate developed and implemented hypothesis-led frameworks at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate conducted primary market research through the development of consumer surveys and interview guides at L.E.K. Consulting&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate worked as a Senior Associate Consultant at Grant Thornton LLP in New York, NY from 2016 to 2018&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate consulted for 10+ clients over 4+ years at Grant Thornton LLP&lt;/fact&gt;\n&lt;fact&gt;Nicholas Pate led data-driven projects using SQL analytics at Grant Thornton LLP&lt;/fact&gt;", "extraction_time": 3.974826, "extraction_model": "gpt-3.5-turbo", "fact_number": 14}</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:09:27.919316</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients 
+• Developed and presented quantitative business cases, influencing key decision-making processes for clients 
+EDUCATION 
+NEW YORK UNIVERSITY, Leonard N. Stern School of Business 
+Master of Business Administration 
+Specializations in Strategy, Business Analytics, and Management 
+New York, NY 
+May 2020 
+• Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club 
+• Member - Stern Technology Association; Management Consulting Association 
+• Teaching Fellow - Digital Strategy; Programming in Python 
+SOUTHWESTERN UNIVERSITY 
+Bachelor of Arts in Business and Economics 
+Georgetown, TX 
+ May 2013 
+• Dean’s List 
+ADDITIONAL INFORMATION 
+• Skills: Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, 
+Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management 
+• Certifications: OpenAI API Bootcamp - Udemy; Intermediate Python for Data Science – DataCamp 
+• Volunteering: Mentor for 15+ middle school, high school, and first-generation college students over 5 different 
+organizations since 2014, providing educational, professional, and personal guidance 
+• Interests: Competitive bowler with ten 300 games, avid musician (singing, piano, and guitar), and coffee roaster</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Developed and presented quantitative business cases, influencing key decision-making processes for clients</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>The submitted fact "Developed and presented quantitative business cases, influencing key decision-making processes for clients" is a valid fact based on the original text. 
+1. The fact directly corresponds to the information provided in the original text about the individual's professional experience.
+2. It names specific activities (developing and presenting quantitative business cases) performed by the individual.
+3. The fact contains a specific, measurable data point related to the individual's work experience.
+4. The context for the fact is complete, mentioning the influence on key decision-making processes for clients.
+5. No additional information is added, and the fact maintains the specific details from the original text.
+6. The fact does not combine information from different parts of the text or make any inferences.
+7. It meets all the criteria for a valid fact as per the verification guidelines.</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>2.883745</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 1729, "timestamp": "2025-02-24T00:09:25.024404"}, "llm_response": "&lt;fact&gt;Consulted for 10+ clients over 4+ years, finding $100M+ in operational improvement opportunities&lt;/fact&gt;\n&lt;fact&gt;Developed and presented quantitative business cases, influencing key decision-making processes for clients&lt;/fact&gt;\n&lt;fact&gt;Master of Business Administration from NEW YORK UNIVERSITY, Leonard N. Stern School of Business&lt;/fact&gt;\n&lt;fact&gt;Specializations in Strategy, Business Analytics, and Management&lt;/fact&gt;\n&lt;fact&gt;Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club&lt;/fact&gt;\n&lt;fact&gt;Member of Stern Technology Association and Management Consulting Association&lt;/fact&gt;\n&lt;fact&gt;Teaching Fellow for Digital Strategy and Programming in Python&lt;/fact&gt;\n&lt;fact&gt;Bachelor of Arts in Business and Economics from SOUTHWESTERN UNIVERSITY&lt;/fact&gt;\n&lt;fact&gt;Dean's List recipient&lt;/fact&gt;\n&lt;fact&gt;Skills include Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management&lt;/fact&gt;\n&lt;fact&gt;Certifications in OpenAI API Bootcamp from Udemy and Intermediate Python for Data Science from DataCamp&lt;/fact&gt;\n&lt;fact&gt;Volunteering experience as a mentor for 15+ students across different organizations since 2014&lt;/fact&gt;\n&lt;fact&gt;Interests include competitive bowling with ten 300 games, music (singing, piano, guitar), and coffee roasting&lt;/fact&gt;", "extraction_time": 2.883745, "extraction_model": "gpt-3.5-turbo", "fact_number": 2}</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:09:27.919329</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients 
+• Developed and presented quantitative business cases, influencing key decision-making processes for clients 
+EDUCATION 
+NEW YORK UNIVERSITY, Leonard N. Stern School of Business 
+Master of Business Administration 
+Specializations in Strategy, Business Analytics, and Management 
+New York, NY 
+May 2020 
+• Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club 
+• Member - Stern Technology Association; Management Consulting Association 
+• Teaching Fellow - Digital Strategy; Programming in Python 
+SOUTHWESTERN UNIVERSITY 
+Bachelor of Arts in Business and Economics 
+Georgetown, TX 
+ May 2013 
+• Dean’s List 
+ADDITIONAL INFORMATION 
+• Skills: Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, 
+Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management 
+• Certifications: OpenAI API Bootcamp - Udemy; Intermediate Python for Data Science – DataCamp 
+• Volunteering: Mentor for 15+ middle school, high school, and first-generation college students over 5 different 
+organizations since 2014, providing educational, professional, and personal guidance 
+• Interests: Competitive bowler with ten 300 games, avid musician (singing, piano, and guitar), and coffee roaster</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Master of Business Administration from NEW YORK UNIVERSITY, Leonard N. Stern School of Business</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>The submitted fact "Master of Business Administration from NEW YORK UNIVERSITY, Leonard N. Stern School of Business" is a valid fact based on the original text. It meets all the verification criteria:
+1. Contains a specific, measurable data point: Master of Business Administration degree.
+2. Names specific entities with their full, proper names: NEW YORK UNIVERSITY, Leonard N. Stern School of Business.
+3. Makes a concrete, testable claim that can be independently verified through the original text.
+4. Matches the original text verbatim.
+5. Contains complete technical context for the measurement.
+6. Includes the unit for the degree (Master of Business Administration).
+7. Specifies the conditions for the measurement (obtained from NEW YORK UNIVERSITY, Leonard N. Stern School of Business).
+8. Does not combine information from different parts of the text.
+9. Does not infer any relationships not explicitly stated.</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>2.883745</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 1729, "timestamp": "2025-02-24T00:09:25.024404"}, "llm_response": "&lt;fact&gt;Consulted for 10+ clients over 4+ years, finding $100M+ in operational improvement opportunities&lt;/fact&gt;\n&lt;fact&gt;Developed and presented quantitative business cases, influencing key decision-making processes for clients&lt;/fact&gt;\n&lt;fact&gt;Master of Business Administration from NEW YORK UNIVERSITY, Leonard N. Stern School of Business&lt;/fact&gt;\n&lt;fact&gt;Specializations in Strategy, Business Analytics, and Management&lt;/fact&gt;\n&lt;fact&gt;Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club&lt;/fact&gt;\n&lt;fact&gt;Member of Stern Technology Association and Management Consulting Association&lt;/fact&gt;\n&lt;fact&gt;Teaching Fellow for Digital Strategy and Programming in Python&lt;/fact&gt;\n&lt;fact&gt;Bachelor of Arts in Business and Economics from SOUTHWESTERN UNIVERSITY&lt;/fact&gt;\n&lt;fact&gt;Dean's List recipient&lt;/fact&gt;\n&lt;fact&gt;Skills include Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management&lt;/fact&gt;\n&lt;fact&gt;Certifications in OpenAI API Bootcamp from Udemy and Intermediate Python for Data Science from DataCamp&lt;/fact&gt;\n&lt;fact&gt;Volunteering experience as a mentor for 15+ students across different organizations since 2014&lt;/fact&gt;\n&lt;fact&gt;Interests include competitive bowling with ten 300 games, music (singing, piano, guitar), and coffee roasting&lt;/fact&gt;", "extraction_time": 2.883745, "extraction_model": "gpt-3.5-turbo", "fact_number": 3}</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:09:27.919747</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients 
+• Developed and presented quantitative business cases, influencing key decision-making processes for clients 
+EDUCATION 
+NEW YORK UNIVERSITY, Leonard N. Stern School of Business 
+Master of Business Administration 
+Specializations in Strategy, Business Analytics, and Management 
+New York, NY 
+May 2020 
+• Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club 
+• Member - Stern Technology Association; Management Consulting Association 
+• Teaching Fellow - Digital Strategy; Programming in Python 
+SOUTHWESTERN UNIVERSITY 
+Bachelor of Arts in Business and Economics 
+Georgetown, TX 
+ May 2013 
+• Dean’s List 
+ADDITIONAL INFORMATION 
+• Skills: Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, 
+Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management 
+• Certifications: OpenAI API Bootcamp - Udemy; Intermediate Python for Data Science – DataCamp 
+• Volunteering: Mentor for 15+ middle school, high school, and first-generation college students over 5 different 
+organizations since 2014, providing educational, professional, and personal guidance 
+• Interests: Competitive bowler with ten 300 games, avid musician (singing, piano, and guitar), and coffee roaster</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Bachelor of Arts in Business and Economics from SOUTHWESTERN UNIVERSITY</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>The submitted fact "Bachelor of Arts in Business and Economics from SOUTHWESTERN UNIVERSITY" can be verified as a valid fact based on the original text. The original text explicitly states the educational background of the individual, mentioning the completion of a Bachelor of Arts in Business and Economics from Southwestern University in May 2013. The fact preserves the specific degree, field of study, and the name of the educational institution without any added inference or missing information. It meets all the criteria for a valid fact as it contains a specific, verifiable data point, names the entity with its full name, and can be directly verified through the original text.</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>2.883745</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 1729, "timestamp": "2025-02-24T00:09:25.024404"}, "llm_response": "&lt;fact&gt;Consulted for 10+ clients over 4+ years, finding $100M+ in operational improvement opportunities&lt;/fact&gt;\n&lt;fact&gt;Developed and presented quantitative business cases, influencing key decision-making processes for clients&lt;/fact&gt;\n&lt;fact&gt;Master of Business Administration from NEW YORK UNIVERSITY, Leonard N. Stern School of Business&lt;/fact&gt;\n&lt;fact&gt;Specializations in Strategy, Business Analytics, and Management&lt;/fact&gt;\n&lt;fact&gt;Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club&lt;/fact&gt;\n&lt;fact&gt;Member of Stern Technology Association and Management Consulting Association&lt;/fact&gt;\n&lt;fact&gt;Teaching Fellow for Digital Strategy and Programming in Python&lt;/fact&gt;\n&lt;fact&gt;Bachelor of Arts in Business and Economics from SOUTHWESTERN UNIVERSITY&lt;/fact&gt;\n&lt;fact&gt;Dean's List recipient&lt;/fact&gt;\n&lt;fact&gt;Skills include Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management&lt;/fact&gt;\n&lt;fact&gt;Certifications in OpenAI API Bootcamp from Udemy and Intermediate Python for Data Science from DataCamp&lt;/fact&gt;\n&lt;fact&gt;Volunteering experience as a mentor for 15+ students across different organizations since 2014&lt;/fact&gt;\n&lt;fact&gt;Interests include competitive bowling with ten 300 games, music (singing, piano, guitar), and coffee roasting&lt;/fact&gt;", "extraction_time": 2.883745, "extraction_model": "gpt-3.5-turbo", "fact_number": 8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:09:27.919776</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients 
+• Developed and presented quantitative business cases, influencing key decision-making processes for clients 
+EDUCATION 
+NEW YORK UNIVERSITY, Leonard N. Stern School of Business 
+Master of Business Administration 
+Specializations in Strategy, Business Analytics, and Management 
+New York, NY 
+May 2020 
+• Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club 
+• Member - Stern Technology Association; Management Consulting Association 
+• Teaching Fellow - Digital Strategy; Programming in Python 
+SOUTHWESTERN UNIVERSITY 
+Bachelor of Arts in Business and Economics 
+Georgetown, TX 
+ May 2013 
+• Dean’s List 
+ADDITIONAL INFORMATION 
+• Skills: Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, 
+Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management 
+• Certifications: OpenAI API Bootcamp - Udemy; Intermediate Python for Data Science – DataCamp 
+• Volunteering: Mentor for 15+ middle school, high school, and first-generation college students over 5 different 
+organizations since 2014, providing educational, professional, and personal guidance 
+• Interests: Competitive bowler with ten 300 games, avid musician (singing, piano, and guitar), and coffee roaster</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Skills include Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>The submitted fact matches the original text verbatim and lists specific skills possessed by the individual, including Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, and Project Management.</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>2.883745</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 1729, "timestamp": "2025-02-24T00:09:25.024404"}, "llm_response": "&lt;fact&gt;Consulted for 10+ clients over 4+ years, finding $100M+ in operational improvement opportunities&lt;/fact&gt;\n&lt;fact&gt;Developed and presented quantitative business cases, influencing key decision-making processes for clients&lt;/fact&gt;\n&lt;fact&gt;Master of Business Administration from NEW YORK UNIVERSITY, Leonard N. Stern School of Business&lt;/fact&gt;\n&lt;fact&gt;Specializations in Strategy, Business Analytics, and Management&lt;/fact&gt;\n&lt;fact&gt;Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club&lt;/fact&gt;\n&lt;fact&gt;Member of Stern Technology Association and Management Consulting Association&lt;/fact&gt;\n&lt;fact&gt;Teaching Fellow for Digital Strategy and Programming in Python&lt;/fact&gt;\n&lt;fact&gt;Bachelor of Arts in Business and Economics from SOUTHWESTERN UNIVERSITY&lt;/fact&gt;\n&lt;fact&gt;Dean's List recipient&lt;/fact&gt;\n&lt;fact&gt;Skills include Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management&lt;/fact&gt;\n&lt;fact&gt;Certifications in OpenAI API Bootcamp from Udemy and Intermediate Python for Data Science from DataCamp&lt;/fact&gt;\n&lt;fact&gt;Volunteering experience as a mentor for 15+ students across different organizations since 2014&lt;/fact&gt;\n&lt;fact&gt;Interests include competitive bowling with ten 300 games, music (singing, piano, guitar), and coffee roasting&lt;/fact&gt;", "extraction_time": 2.883745, "extraction_model": "gpt-3.5-turbo", "fact_number": 10}</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:09:27.919789</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients 
+• Developed and presented quantitative business cases, influencing key decision-making processes for clients 
+EDUCATION 
+NEW YORK UNIVERSITY, Leonard N. Stern School of Business 
+Master of Business Administration 
+Specializations in Strategy, Business Analytics, and Management 
+New York, NY 
+May 2020 
+• Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club 
+• Member - Stern Technology Association; Management Consulting Association 
+• Teaching Fellow - Digital Strategy; Programming in Python 
+SOUTHWESTERN UNIVERSITY 
+Bachelor of Arts in Business and Economics 
+Georgetown, TX 
+ May 2013 
+• Dean’s List 
+ADDITIONAL INFORMATION 
+• Skills: Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, 
+Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management 
+• Certifications: OpenAI API Bootcamp - Udemy; Intermediate Python for Data Science – DataCamp 
+• Volunteering: Mentor for 15+ middle school, high school, and first-generation college students over 5 different 
+organizations since 2014, providing educational, professional, and personal guidance 
+• Interests: Competitive bowler with ten 300 games, avid musician (singing, piano, and guitar), and coffee roaster</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Certifications in OpenAI API Bootcamp from Udemy and Intermediate Python for Data Science from DataCamp</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>The submitted fact is a valid fact based on the original text. It directly matches the information provided in the "ADDITIONAL INFORMATION" section regarding the certifications obtained by the individual. The fact preserves the specific certifications mentioned, "OpenAI API Bootcamp - Udemy" and "Intermediate Python for Data Science – DataCamp," without adding any new information or inference. The fact contains specific, verifiable data points about the individual's certifications.</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>2.883745</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 1729, "timestamp": "2025-02-24T00:09:25.024404"}, "llm_response": "&lt;fact&gt;Consulted for 10+ clients over 4+ years, finding $100M+ in operational improvement opportunities&lt;/fact&gt;\n&lt;fact&gt;Developed and presented quantitative business cases, influencing key decision-making processes for clients&lt;/fact&gt;\n&lt;fact&gt;Master of Business Administration from NEW YORK UNIVERSITY, Leonard N. Stern School of Business&lt;/fact&gt;\n&lt;fact&gt;Specializations in Strategy, Business Analytics, and Management&lt;/fact&gt;\n&lt;fact&gt;Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club&lt;/fact&gt;\n&lt;fact&gt;Member of Stern Technology Association and Management Consulting Association&lt;/fact&gt;\n&lt;fact&gt;Teaching Fellow for Digital Strategy and Programming in Python&lt;/fact&gt;\n&lt;fact&gt;Bachelor of Arts in Business and Economics from SOUTHWESTERN UNIVERSITY&lt;/fact&gt;\n&lt;fact&gt;Dean's List recipient&lt;/fact&gt;\n&lt;fact&gt;Skills include Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management&lt;/fact&gt;\n&lt;fact&gt;Certifications in OpenAI API Bootcamp from Udemy and Intermediate Python for Data Science from DataCamp&lt;/fact&gt;\n&lt;fact&gt;Volunteering experience as a mentor for 15+ students across different organizations since 2014&lt;/fact&gt;\n&lt;fact&gt;Interests include competitive bowling with ten 300 games, music (singing, piano, guitar), and coffee roasting&lt;/fact&gt;", "extraction_time": 2.883745, "extraction_model": "gpt-3.5-turbo", "fact_number": 11}</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:09:27.919802</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients 
+• Developed and presented quantitative business cases, influencing key decision-making processes for clients 
+EDUCATION 
+NEW YORK UNIVERSITY, Leonard N. Stern School of Business 
+Master of Business Administration 
+Specializations in Strategy, Business Analytics, and Management 
+New York, NY 
+May 2020 
+• Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club 
+• Member - Stern Technology Association; Management Consulting Association 
+• Teaching Fellow - Digital Strategy; Programming in Python 
+SOUTHWESTERN UNIVERSITY 
+Bachelor of Arts in Business and Economics 
+Georgetown, TX 
+ May 2013 
+• Dean’s List 
+ADDITIONAL INFORMATION 
+• Skills: Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, 
+Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management 
+• Certifications: OpenAI API Bootcamp - Udemy; Intermediate Python for Data Science – DataCamp 
+• Volunteering: Mentor for 15+ middle school, high school, and first-generation college students over 5 different 
+organizations since 2014, providing educational, professional, and personal guidance 
+• Interests: Competitive bowler with ten 300 games, avid musician (singing, piano, and guitar), and coffee roaster</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Volunteering experience as a mentor for 15+ students across different organizations since 2014</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>The submitted fact accurately reflects the volunteering experience mentioned in the original text. The statement specifically mentions mentoring 15+ students across different organizations since 2014, which is a quantifiable and verifiable data point directly extracted from the original text.</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>2.883745</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 1729, "timestamp": "2025-02-24T00:09:25.024404"}, "llm_response": "&lt;fact&gt;Consulted for 10+ clients over 4+ years, finding $100M+ in operational improvement opportunities&lt;/fact&gt;\n&lt;fact&gt;Developed and presented quantitative business cases, influencing key decision-making processes for clients&lt;/fact&gt;\n&lt;fact&gt;Master of Business Administration from NEW YORK UNIVERSITY, Leonard N. Stern School of Business&lt;/fact&gt;\n&lt;fact&gt;Specializations in Strategy, Business Analytics, and Management&lt;/fact&gt;\n&lt;fact&gt;Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club&lt;/fact&gt;\n&lt;fact&gt;Member of Stern Technology Association and Management Consulting Association&lt;/fact&gt;\n&lt;fact&gt;Teaching Fellow for Digital Strategy and Programming in Python&lt;/fact&gt;\n&lt;fact&gt;Bachelor of Arts in Business and Economics from SOUTHWESTERN UNIVERSITY&lt;/fact&gt;\n&lt;fact&gt;Dean's List recipient&lt;/fact&gt;\n&lt;fact&gt;Skills include Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management&lt;/fact&gt;\n&lt;fact&gt;Certifications in OpenAI API Bootcamp from Udemy and Intermediate Python for Data Science from DataCamp&lt;/fact&gt;\n&lt;fact&gt;Volunteering experience as a mentor for 15+ students across different organizations since 2014&lt;/fact&gt;\n&lt;fact&gt;Interests include competitive bowling with ten 300 games, music (singing, piano, guitar), and coffee roasting&lt;/fact&gt;", "extraction_time": 2.883745, "extraction_model": "gpt-3.5-turbo", "fact_number": 12}</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-02-24T00:09:27.919816</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>file:///Users/nicho/Documents/Nicholas_Pate_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>New York, NY 
+2016 - 2018 
+2014-2016 
+• Consulted for 10+ clients over 4+ years, interacting with client personnel, managing Associates, and providing heavy 
+analytical skills to solve client problems, ultimately finding $100M+ in operational improvement opportunities 
+• Led data-driven projects using SQL analytics, uncovering significant supply chain and profit improvement 
+opportunities for clients 
+• Developed and presented quantitative business cases, influencing key decision-making processes for clients 
+EDUCATION 
+NEW YORK UNIVERSITY, Leonard N. Stern School of Business 
+Master of Business Administration 
+Specializations in Strategy, Business Analytics, and Management 
+New York, NY 
+May 2020 
+• Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club 
+• Member - Stern Technology Association; Management Consulting Association 
+• Teaching Fellow - Digital Strategy; Programming in Python 
+SOUTHWESTERN UNIVERSITY 
+Bachelor of Arts in Business and Economics 
+Georgetown, TX 
+ May 2013 
+• Dean’s List 
+ADDITIONAL INFORMATION 
+• Skills: Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, 
+Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management 
+• Certifications: OpenAI API Bootcamp - Udemy; Intermediate Python for Data Science – DataCamp 
+• Volunteering: Mentor for 15+ middle school, high school, and first-generation college students over 5 different 
+organizations since 2014, providing educational, professional, and personal guidance 
+• Interests: Competitive bowler with ten 300 games, avid musician (singing, piano, and guitar), and coffee roaster</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Interests include competitive bowling with ten 300 games, music (singing, piano, guitar), and coffee roasting</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>verified</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>The submitted fact accurately reflects the information provided in the original text without any added inference or missing details. It specifically mentions the individual's interests as competitive bowling with ten 300 games, music involving singing, piano, and guitar, as well as coffee roasting. These details are directly verifiable from the original text.</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>2.883745</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>{"chunk_metadata": {"char_length": 1729, "timestamp": "2025-02-24T00:09:25.024404"}, "llm_response": "&lt;fact&gt;Consulted for 10+ clients over 4+ years, finding $100M+ in operational improvement opportunities&lt;/fact&gt;\n&lt;fact&gt;Developed and presented quantitative business cases, influencing key decision-making processes for clients&lt;/fact&gt;\n&lt;fact&gt;Master of Business Administration from NEW YORK UNIVERSITY, Leonard N. Stern School of Business&lt;/fact&gt;\n&lt;fact&gt;Specializations in Strategy, Business Analytics, and Management&lt;/fact&gt;\n&lt;fact&gt;Leadership Positions - Associate WP of Academics, Business Analytics Club; VP of Events, Business Analytics Club&lt;/fact&gt;\n&lt;fact&gt;Member of Stern Technology Association and Management Consulting Association&lt;/fact&gt;\n&lt;fact&gt;Teaching Fellow for Digital Strategy and Programming in Python&lt;/fact&gt;\n&lt;fact&gt;Bachelor of Arts in Business and Economics from SOUTHWESTERN UNIVERSITY&lt;/fact&gt;\n&lt;fact&gt;Dean's List recipient&lt;/fact&gt;\n&lt;fact&gt;Skills include Python, SQL, Generative AI, APIs, Business Analytics, Data Analysis, Qualitative Research, Strategy, Consulting, Market Research, Stakeholder Interviews, Leadership, Team Management, Project Management&lt;/fact&gt;\n&lt;fact&gt;Certifications in OpenAI API Bootcamp from Udemy and Intermediate Python for Data Science from DataCamp&lt;/fact&gt;\n&lt;fact&gt;Volunteering experience as a mentor for 15+ students across different organizations since 2014&lt;/fact&gt;\n&lt;fact&gt;Interests include competitive bowling with ten 300 games, music (singing, piano, guitar), and coffee roasting&lt;/fact&gt;", "extraction_time": 2.883745, "extraction_model": "gpt-3.5-turbo", "fact_number": 13}</t>
         </is>
       </c>
     </row>

</xml_diff>